<commit_message>
Updated 1 test case test data after test execution findings
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_PanelAccessories_Pro_Lite_Panels.xlsx
+++ b/Test Data/Gallery_PanelAccessories_Pro_Lite_Panels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382BCCD1-5C5C-4DA5-84D3-109B9D7EC839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F254FF4-8928-4E4C-8158-A618BC7FCBBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="25">
   <si>
     <t>Wg</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>FB800</t>
-  </si>
-  <si>
-    <t>PCS800</t>
   </si>
   <si>
     <t>POS800-M</t>
@@ -563,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -585,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -613,22 +610,22 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -702,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -730,17 +727,17 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -768,7 +765,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -814,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -842,17 +839,17 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,7 +877,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -926,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -949,22 +946,22 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1016,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1038,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -1066,17 +1063,17 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>